<commit_message>
tests for creating businesss account with lcoations, domainas, etc from excel
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Domenii existente" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Servicii" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Angajati" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Permisiuni" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
@@ -59,6 +60,46 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -98,6 +139,46 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -137,6 +218,46 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -178,6 +299,36 @@
     <author/>
   </authors>
   <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Domeniu principal
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Domeniu principal
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B1" authorId="0">
       <text>
         <r>
@@ -221,7 +372,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="145">
   <si>
     <t>Categorie Afacere</t>
   </si>
@@ -304,16 +455,16 @@
     <t>Educație </t>
   </si>
   <si>
-    <t>Scoala particulara Curcubeu</t>
-  </si>
-  <si>
-    <t>grigotontea@automation.33mail.com</t>
-  </si>
-  <si>
-    <t>str Aurora boreala nr 5</t>
-  </si>
-  <si>
-    <t>0265444111</t>
+    <t>Scoala particulara Ghicel</t>
+  </si>
+  <si>
+    <t>ghiocelprimavaraa@automation.33mail.com</t>
+  </si>
+  <si>
+    <t>str Morariei nr 10</t>
+  </si>
+  <si>
+    <t>0264888641</t>
   </si>
   <si>
     <t>Imobiliare </t>
@@ -349,28 +500,28 @@
     <t>Telefon receptionist</t>
   </si>
   <si>
-    <t>Ioana</t>
-  </si>
-  <si>
-    <t>ioana_1@staffcalendis.33mail.com</t>
+    <t>Rubarba Mihaelaa</t>
+  </si>
+  <si>
+    <t>receptionsis112a@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0264555887</t>
   </si>
   <si>
-    <t>Praslea</t>
-  </si>
-  <si>
-    <t>praslea_1@staffcalendis.33mail.com.</t>
+    <t>Venula Mihaila</t>
+  </si>
+  <si>
+    <t>receptionist113@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0261111222</t>
   </si>
   <si>
-    <t>Carpacio</t>
-  </si>
-  <si>
-    <t>carapacio@staffcalendis.33mail.com</t>
+    <t>NilaStefania</t>
+  </si>
+  <si>
+    <t>receptionsits114@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0268774112</t>
@@ -412,7 +563,7 @@
     <t>Duminica</t>
   </si>
   <si>
-    <t>Str hateg 28</t>
+    <t>Str Fraternitatii nr 7</t>
   </si>
   <si>
     <t>Cluj</t>
@@ -421,43 +572,61 @@
     <t>Cluj-Napoca</t>
   </si>
   <si>
-    <t>0264555441</t>
-  </si>
-  <si>
-    <t>Sediu Horea</t>
+    <t>0264555141</t>
+  </si>
+  <si>
+    <t>Sediu Flying</t>
+  </si>
+  <si>
+    <t>10:00-20:00</t>
+  </si>
+  <si>
+    <t>10:00-14:00</t>
+  </si>
+  <si>
+    <t>inchis</t>
+  </si>
+  <si>
+    <t>str Coloar 89</t>
+  </si>
+  <si>
+    <t>Alba</t>
+  </si>
+  <si>
+    <t>Alba Iulia</t>
+  </si>
+  <si>
+    <t>0263555441</t>
+  </si>
+  <si>
+    <t>Sediu Alba</t>
+  </si>
+  <si>
+    <t>9:00-17:00</t>
+  </si>
+  <si>
+    <t>9:00-21:00</t>
+  </si>
+  <si>
+    <t>9:00-15:00</t>
+  </si>
+  <si>
+    <t>str Alexadru Mircea nr 69</t>
+  </si>
+  <si>
+    <t>0254111222</t>
+  </si>
+  <si>
+    <t>Sediu Romulus</t>
   </si>
   <si>
     <t>9:00-12:00</t>
   </si>
   <si>
-    <t>9:00-17:00</t>
-  </si>
-  <si>
-    <t>10:00-15:00</t>
-  </si>
-  <si>
-    <t>inchis</t>
-  </si>
-  <si>
-    <t>str dorului 78</t>
-  </si>
-  <si>
-    <t>Alba</t>
-  </si>
-  <si>
-    <t>Oiejdea</t>
-  </si>
-  <si>
-    <t>0263555448</t>
-  </si>
-  <si>
-    <t>Sediu Alba</t>
-  </si>
-  <si>
-    <t>str martisorului nr 5</t>
-  </si>
-  <si>
-    <t>0254111223</t>
+    <t>10:00-19:00</t>
+  </si>
+  <si>
+    <t>10:00-18:00</t>
   </si>
   <si>
     <t>Nume domeniu</t>
@@ -466,13 +635,13 @@
     <t>Locatia domeniului</t>
   </si>
   <si>
-    <t>after school</t>
-  </si>
-  <si>
-    <t>Scoala 1-5</t>
-  </si>
-  <si>
-    <t>Scoala 5-8</t>
+    <t>scoala</t>
+  </si>
+  <si>
+    <t>playing</t>
+  </si>
+  <si>
+    <t>art activities</t>
   </si>
   <si>
     <t>Bronzare organica </t>
@@ -532,16 +701,16 @@
     <t>Persoane serviciu</t>
   </si>
   <si>
-    <t>homework</t>
-  </si>
-  <si>
-    <t>playing</t>
-  </si>
-  <si>
-    <t>math</t>
-  </si>
-  <si>
-    <t>biology</t>
+    <t>teme acasa</t>
+  </si>
+  <si>
+    <t>darts</t>
+  </si>
+  <si>
+    <t>pictura</t>
+  </si>
+  <si>
+    <t>jocuri logica</t>
   </si>
   <si>
     <t>100.66</t>
@@ -556,10 +725,13 @@
     <t>Telefon angajat</t>
   </si>
   <si>
-    <t>Ruxandra</t>
-  </si>
-  <si>
-    <t>ruxandra@staffcalendis.33mail.com</t>
+    <t>Serviciu asignat</t>
+  </si>
+  <si>
+    <t>Scolpol Maria</t>
+  </si>
+  <si>
+    <t>angaja112a@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0264555112</t>
@@ -571,22 +743,70 @@
     <t>10:00-17:00</t>
   </si>
   <si>
-    <t>Nichita</t>
-  </si>
-  <si>
-    <t>oliacn@staffcalendis.33mail.com</t>
+    <t>Mobutu seseku</t>
+  </si>
+  <si>
+    <t>angajata113a@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0264111887</t>
   </si>
   <si>
-    <t>Camila</t>
-  </si>
-  <si>
-    <t>camilacamilla@staffcalendis.33mail.com</t>
+    <t>Moceal Rapil</t>
+  </si>
+  <si>
+    <t>dsfsdgajatasdfs114a@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0265444112</t>
+  </si>
+  <si>
+    <t>Spiral Agar</t>
+  </si>
+  <si>
+    <t>Ldfkvgdlsf65115@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>10:00-21:00</t>
+  </si>
+  <si>
+    <t>9:00-18:30</t>
+  </si>
+  <si>
+    <t>Creare programari</t>
+  </si>
+  <si>
+    <t>Modificari programari in viitor</t>
+  </si>
+  <si>
+    <t>Modificari programari in trecut</t>
+  </si>
+  <si>
+    <t>Vizualizare calendar</t>
+  </si>
+  <si>
+    <t>Creare programari alti specialisti</t>
+  </si>
+  <si>
+    <t>Modificari programari in viitor alti specialisti</t>
+  </si>
+  <si>
+    <t>Modificari programari in trecut alti specialisti</t>
+  </si>
+  <si>
+    <t>Date de contact clienti</t>
+  </si>
+  <si>
+    <t>Vizualizare baza de date clienti</t>
+  </si>
+  <si>
+    <t>Editare informatii clienti</t>
+  </si>
+  <si>
+    <t>Setari orar</t>
+  </si>
+  <si>
+    <t>Setari exceptii</t>
   </si>
 </sst>
 </file>
@@ -598,7 +818,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -660,6 +880,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FFFF3333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -706,7 +934,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -759,6 +987,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -804,7 +1040,7 @@
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFF3333"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
@@ -868,15 +1104,15 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1070,13 +1306,14 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1090,7 +1327,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>42</v>
       </c>
@@ -1101,7 +1338,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
         <v>45</v>
       </c>
@@ -1112,7 +1349,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>48</v>
       </c>
@@ -1124,11 +1361,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="ioana_1@staffcalendis.33mail.com"/>
-    <hyperlink ref="B3" r:id="rId2" display="praslea_1@staffcalendis.33mail.com."/>
-    <hyperlink ref="B4" r:id="rId3" display="carapacio@staffcalendis.33mail.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1147,16 +1379,16 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1217,65 +1449,65 @@
         <v>68</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>68</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>69</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>69</v>
-      </c>
       <c r="G3" s="0" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>64</v>
@@ -1284,31 +1516,31 @@
         <v>65</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1330,25 +1562,26 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9489795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>67</v>
@@ -1356,35 +1589,47 @@
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="n">
         <v>0.0625</v>
       </c>
+      <c r="B4" s="0" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="n">
         <v>0.0833333333333333</v>
       </c>
+      <c r="B5" s="0" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="n">
         <v>0.104166666666667</v>
       </c>
+      <c r="B6" s="0" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="n">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>67</v>
@@ -1478,72 +1723,72 @@
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="2" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1573,41 +1818,42 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>81</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>30</v>
@@ -1619,12 +1865,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>81</v>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>30</v>
@@ -1636,12 +1882,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>82</v>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>89</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>20</v>
@@ -1653,26 +1899,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>83</v>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>60</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E5" s="12" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A4">
+  <conditionalFormatting sqref="A2:A3">
     <cfRule type="cellIs" priority="2" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>9:0</formula>
+      <formula>17:0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="cellIs" priority="3" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>9:0</formula>
       <formula>17:0</formula>
     </cfRule>
@@ -1693,7 +1945,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
@@ -1701,22 +1953,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.5561224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>56</v>
@@ -1739,104 +1991,154 @@
       <c r="J1" s="0" t="s">
         <v>62</v>
       </c>
+      <c r="K1" s="13" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId2" display="Ldfkvgdlsf65115@staffcalendis"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1844,6 +2146,223 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new schedule to read for tests
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Cont adminstrator" sheetId="1" state="visible" r:id="rId2"/>
@@ -100,6 +100,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -179,6 +181,8 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -258,6 +262,8 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -455,10 +461,10 @@
     <t>Educație </t>
   </si>
   <si>
-    <t>Scoala particulara Ghicel</t>
-  </si>
-  <si>
-    <t>ghiocelprimavaraa@automation.33mail.com</t>
+    <t>Scoala particulara Boboc</t>
+  </si>
+  <si>
+    <t>bobocscoala@automation.33mail.com</t>
   </si>
   <si>
     <t>str Morariei nr 10</t>
@@ -731,7 +737,7 @@
     <t>Scolpol Maria</t>
   </si>
   <si>
-    <t>angaja112a@staffcalendis.33mail.com</t>
+    <t>maria1111@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0264555112</t>
@@ -746,7 +752,7 @@
     <t>Mobutu seseku</t>
   </si>
   <si>
-    <t>angajata113a@staffcalendis.33mail.com</t>
+    <t>seseku1112@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0264111887</t>
@@ -755,7 +761,7 @@
     <t>Moceal Rapil</t>
   </si>
   <si>
-    <t>dsfsdgajatasdfs114a@staffcalendis.33mail.com</t>
+    <t>ralph1113@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0265444112</t>
@@ -764,7 +770,7 @@
     <t>Spiral Agar</t>
   </si>
   <si>
-    <t>Ldfkvgdlsf65115@staffcalendis.33mail.com</t>
+    <t>spiral1114@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>10:00-21:00</t>
@@ -1103,16 +1109,16 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1311,9 +1317,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1384,11 +1391,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1567,8 +1575,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1667,6 +1676,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
@@ -1823,12 +1835,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.10204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1947,17 +1960,20 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2137,7 +2153,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId2" display="Ldfkvgdlsf65115@staffcalendis"/>
+    <hyperlink ref="B5" r:id="rId2" display="spiral1114@staffcalendis.33mail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2162,9 +2178,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">

</xml_diff>

<commit_message>
new xlsx file test data
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="974" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="974" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cont adminstrator" sheetId="1" state="visible" r:id="rId2"/>
@@ -104,6 +104,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -187,6 +188,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -270,6 +272,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -459,10 +462,10 @@
     <t>Educație</t>
   </si>
   <si>
-    <t>Scoala particulara Vecverita</t>
-  </si>
-  <si>
-    <t>veveritascoala@automation.33mail.com</t>
+    <t>Scoala particulara Moira</t>
+  </si>
+  <si>
+    <t>moirascoala@automation.33mail.com</t>
   </si>
   <si>
     <t>str Morariei nr 10</t>
@@ -507,7 +510,7 @@
     <t>Rubarba Mihaelaa</t>
   </si>
   <si>
-    <t>steluta2a@staffcalendis.33mail.com</t>
+    <t>steluta2a1@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0264555887</t>
@@ -516,7 +519,7 @@
     <t>Venula Mihaila</t>
   </si>
   <si>
-    <t>steluta313@staffcalendis.33mail.com</t>
+    <t>steluta3131a@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0261111222</t>
@@ -525,7 +528,7 @@
     <t>NilaStefania</t>
   </si>
   <si>
-    <t>steluta44@staffcalendis.33mail.com</t>
+    <t>steluta441a@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0268774112</t>
@@ -735,7 +738,7 @@
     <t>Scolpol Maria</t>
   </si>
   <si>
-    <t>elenas111@staffcalendis.33mail.com</t>
+    <t>elenas1114@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0264555112</t>
@@ -750,7 +753,7 @@
     <t>Mobutu seseku</t>
   </si>
   <si>
-    <t>komornic112@staffcalendis.33mail.com</t>
+    <t>komornic1124@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0264111887</t>
@@ -759,7 +762,7 @@
     <t>Moceal Rapil</t>
   </si>
   <si>
-    <t>ovidius13@staffcalendis.33mail.com</t>
+    <t>ovidius134@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0265444112</t>
@@ -768,7 +771,7 @@
     <t>Spiral Agar</t>
   </si>
   <si>
-    <t>roses4@staffcalendis.33mail.com</t>
+    <t>sdroses4@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>10:00-21:00</t>
@@ -1103,7 +1106,7 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1306,8 +1309,8 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1956,7 +1959,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2111,7 +2114,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>129</v>
       </c>
@@ -2147,9 +2150,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId2" display="roses4@staffcalendis.33mail.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2157,7 +2157,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated chrome to headless run
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cont adminstrator" sheetId="1" state="visible" r:id="rId2"/>
@@ -106,6 +106,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -191,6 +192,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -276,6 +278,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -470,10 +473,10 @@
     <t xml:space="preserve">Educație</t>
   </si>
   <si>
-    <t xml:space="preserve">Scoala particulara Scalpol M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scalpolscoala@automation.33mail.com</t>
+    <t xml:space="preserve">Scoala particulara Mario M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marioscaola1@automation.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">str Morariei nr 10</t>
@@ -518,7 +521,7 @@
     <t xml:space="preserve">Rubarba Mihaelaa</t>
   </si>
   <si>
-    <t xml:space="preserve">steluta2a1@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">steluta2za1@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264555887</t>
@@ -527,7 +530,7 @@
     <t xml:space="preserve">Venula Mihaila</t>
   </si>
   <si>
-    <t xml:space="preserve">steluta3131a@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">steluta3131za@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0261111222</t>
@@ -536,7 +539,7 @@
     <t xml:space="preserve">NilaStefania</t>
   </si>
   <si>
-    <t xml:space="preserve">steluta441a@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">steluta441za@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0268774112</t>
@@ -746,7 +749,7 @@
     <t xml:space="preserve">Scolpol Maria</t>
   </si>
   <si>
-    <t xml:space="preserve">elenaz114@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">elenaz114a1@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264555112</t>
@@ -761,7 +764,7 @@
     <t xml:space="preserve">Mobutu seseku</t>
   </si>
   <si>
-    <t xml:space="preserve">komornicz1124@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">komornicza11124@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264111887</t>
@@ -770,7 +773,7 @@
     <t xml:space="preserve">Moceal Rapil</t>
   </si>
   <si>
-    <t xml:space="preserve">ovidiusz134@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">ovidiusz11a34@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0265444112</t>
@@ -779,7 +782,7 @@
     <t xml:space="preserve">Spiral Agar</t>
   </si>
   <si>
-    <t xml:space="preserve">sdrosesz4@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">sdrosea1sz4@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">10:00-21:00</t>
@@ -1026,9 +1029,9 @@
         <name val="Calibri"/>
         <charset val="1"/>
         <family val="2"/>
-        <color rgb="FF0563C1"/>
-        <u val="single"/>
+        <color rgb="FF000000"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -1121,7 +1124,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.24696356275304"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.35627530364373"/>
   </cols>
@@ -1316,15 +1319,15 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.0607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.4898785425101"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.35627530364373"/>
   </cols>
   <sheetData>
@@ -1396,11 +1399,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.96356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.63967611336032"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.35627530364373"/>
   </cols>
   <sheetData>
@@ -1580,8 +1583,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.35627530364373"/>
   </cols>
   <sheetData>
@@ -1840,8 +1843,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.1417004048583"/>
@@ -1965,19 +1968,19 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2429149797571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4574898785425"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.24696356275304"/>
     <col collapsed="false" hidden="false" max="10" min="7" style="0" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.35627530364373"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
updated iulia xlsx file
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cont adminstrator" sheetId="1" state="visible" r:id="rId2"/>
@@ -108,6 +108,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -195,6 +196,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -282,6 +284,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -308,7 +311,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Domeniu principal</t>
+          <t>Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -332,7 +335,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Domeniu principal</t>
+          <t>Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -346,7 +349,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Domeniu principal</t>
+          <t>Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -360,7 +363,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">*serviciile trebuie sa apartina neaparat de un domeniu</t>
+          <t>*serviciile trebuie sa apartina neaparat de un domeniu</t>
         </r>
       </text>
     </comment>
@@ -384,7 +387,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">* se pot adauga oricate conturi de angajati doriti</t>
+          <t>* se pot adauga oricate conturi de angajati doriti</t>
         </r>
       </text>
     </comment>
@@ -395,439 +398,439 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="145">
   <si>
-    <t xml:space="preserve">Categorie Afacere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume Afacere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email Cont Administrator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adresa afacere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon afacere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medicină dentară</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frumusețe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Larissa's style</t>
-  </si>
-  <si>
-    <t xml:space="preserve">larissa@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calea Martirilor 127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0263221114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medicină</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Animale de companie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sport și agrement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terapii complementare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instalații</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regomart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regomart@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Piata Mare 45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555113</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juridic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resurse umane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asigurări</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modă și îmbrăcăminte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organizare evenimente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Educație</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scoala particulara Mario M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">marioscaola1@automation.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">str Morariei nr 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264888641</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imobiliare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bebeco Adeco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bebbeco@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aleea Bucura 46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0254888777</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reparații</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Psihologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Altă categorie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume receptionist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email receptionist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon receptionist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rubarba Mihaelaa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">steluta2za1@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555887</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venula Mihaila</t>
-  </si>
-  <si>
-    <t xml:space="preserve">steluta3131zza@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0261111222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NilaStefania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">steluta441za@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0268774112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adresa locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Judet locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Localitate locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miercuri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vineri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sambata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duminica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Str Fraternitatii nr 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cluj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cluj-Napoca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555141</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediu Flying</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-20:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-14:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inchis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">str Coloar 89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alba Iulia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0263555441</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediu Alba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-17:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-21:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-15:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">str Alexadru Mircea nr 69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0254111222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediu Romulus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-12:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-19:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-18:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume domeniu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Locatia domeniului</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scoala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">playing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">art activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bronzare organica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chirurgie estetica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coafor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cosmetica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epilare definitiva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frizerie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Make-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manichiura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Masaj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pedichiura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remodelare corporala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tatuaje&amp;piercing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Domeniul asociat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serviciu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durata serviciu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pret serviciu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Persoane serviciu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teme acasa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">darts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pictura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jocuri logica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100.66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume angajat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email angajat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon angajat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serviciu asignat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scolpol Maria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elenaz114a1@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-13:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-17:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobutu seseku</t>
-  </si>
-  <si>
-    <t xml:space="preserve">komornicza11124@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264111887</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moceal Rapil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ovidiusz11a34@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0265444112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spiral Agar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdrosea1sz4@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-21:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-18:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creare programari</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificari programari in viitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificari programari in trecut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vizualizare calendar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creare programari alti specialisti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificari programari in viitor alti specialisti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificari programari in trecut alti specialisti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date de contact clienti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vizualizare baza de date clienti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Editare informatii clienti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setari orar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setari exceptii</t>
+    <t>Categorie Afacere</t>
+  </si>
+  <si>
+    <t>Nume Afacere</t>
+  </si>
+  <si>
+    <t>Email Cont Administrator</t>
+  </si>
+  <si>
+    <t>Adresa afacere</t>
+  </si>
+  <si>
+    <t>Telefon afacere</t>
+  </si>
+  <si>
+    <t>Medicină dentară</t>
+  </si>
+  <si>
+    <t>Frumusețe</t>
+  </si>
+  <si>
+    <t>Larissa's style</t>
+  </si>
+  <si>
+    <t>larissa@yopmail.com</t>
+  </si>
+  <si>
+    <t>Calea Martirilor 127</t>
+  </si>
+  <si>
+    <t>0263221114</t>
+  </si>
+  <si>
+    <t>Medicină</t>
+  </si>
+  <si>
+    <t>Animale de companie</t>
+  </si>
+  <si>
+    <t>Sport și agrement</t>
+  </si>
+  <si>
+    <t>Terapii complementare</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>Instalații</t>
+  </si>
+  <si>
+    <t>Regomart</t>
+  </si>
+  <si>
+    <t>regomart@yopmail.com</t>
+  </si>
+  <si>
+    <t>Piata Mare 45</t>
+  </si>
+  <si>
+    <t>0264555113</t>
+  </si>
+  <si>
+    <t>Juridic</t>
+  </si>
+  <si>
+    <t>Resurse umane</t>
+  </si>
+  <si>
+    <t>Asigurări</t>
+  </si>
+  <si>
+    <t>Modă și îmbrăcăminte</t>
+  </si>
+  <si>
+    <t>Organizare evenimente</t>
+  </si>
+  <si>
+    <t>Educație</t>
+  </si>
+  <si>
+    <t>Scoala particulara Mario M</t>
+  </si>
+  <si>
+    <t>marioscaola1@automation.33mail.com</t>
+  </si>
+  <si>
+    <t>str Morariei nr 10</t>
+  </si>
+  <si>
+    <t>0264888641</t>
+  </si>
+  <si>
+    <t>Imobiliare</t>
+  </si>
+  <si>
+    <t>Bebeco Adeco</t>
+  </si>
+  <si>
+    <t>bebbeco@yopmail.com</t>
+  </si>
+  <si>
+    <t>Aleea Bucura 46</t>
+  </si>
+  <si>
+    <t>0254888777</t>
+  </si>
+  <si>
+    <t>Reparații</t>
+  </si>
+  <si>
+    <t>Psihologie</t>
+  </si>
+  <si>
+    <t>Altă categorie</t>
+  </si>
+  <si>
+    <t>Nume receptionist</t>
+  </si>
+  <si>
+    <t>Email receptionist</t>
+  </si>
+  <si>
+    <t>Telefon receptionist</t>
+  </si>
+  <si>
+    <t>Rubarba Mihaelaa</t>
+  </si>
+  <si>
+    <t>steluta2za1@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0264555887</t>
+  </si>
+  <si>
+    <t>Venula Mihaila</t>
+  </si>
+  <si>
+    <t>steluta3131zzdda@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0261111222</t>
+  </si>
+  <si>
+    <t>NilaStefania</t>
+  </si>
+  <si>
+    <t>steluta441za@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0268774112</t>
+  </si>
+  <si>
+    <t>Adresa locatie</t>
+  </si>
+  <si>
+    <t>Judet locatie</t>
+  </si>
+  <si>
+    <t>Localitate locatie</t>
+  </si>
+  <si>
+    <t>Telefon locatie</t>
+  </si>
+  <si>
+    <t>Nume locatie</t>
+  </si>
+  <si>
+    <t>Luni</t>
+  </si>
+  <si>
+    <t>Marti</t>
+  </si>
+  <si>
+    <t>Miercuri</t>
+  </si>
+  <si>
+    <t>Joi</t>
+  </si>
+  <si>
+    <t>Vineri</t>
+  </si>
+  <si>
+    <t>Sambata</t>
+  </si>
+  <si>
+    <t>Duminica</t>
+  </si>
+  <si>
+    <t>Str Fraternitatii nr 7</t>
+  </si>
+  <si>
+    <t>Cluj</t>
+  </si>
+  <si>
+    <t>Cluj-Napoca</t>
+  </si>
+  <si>
+    <t>0264555141</t>
+  </si>
+  <si>
+    <t>Sediu Flying</t>
+  </si>
+  <si>
+    <t>10:00-20:00</t>
+  </si>
+  <si>
+    <t>10:00-14:00</t>
+  </si>
+  <si>
+    <t>inchis</t>
+  </si>
+  <si>
+    <t>str Coloar 89</t>
+  </si>
+  <si>
+    <t>Alba</t>
+  </si>
+  <si>
+    <t>Alba Iulia</t>
+  </si>
+  <si>
+    <t>0263555441</t>
+  </si>
+  <si>
+    <t>Sediu Alba</t>
+  </si>
+  <si>
+    <t>9:00-17:00</t>
+  </si>
+  <si>
+    <t>9:00-21:00</t>
+  </si>
+  <si>
+    <t>9:00-15:00</t>
+  </si>
+  <si>
+    <t>str Alexadru Mircea nr 69</t>
+  </si>
+  <si>
+    <t>0254111222</t>
+  </si>
+  <si>
+    <t>Sediu Romulus</t>
+  </si>
+  <si>
+    <t>9:00-12:00</t>
+  </si>
+  <si>
+    <t>10:00-19:00</t>
+  </si>
+  <si>
+    <t>10:00-18:00</t>
+  </si>
+  <si>
+    <t>Nume domeniu</t>
+  </si>
+  <si>
+    <t>Locatia domeniului</t>
+  </si>
+  <si>
+    <t>scoala</t>
+  </si>
+  <si>
+    <t>playing</t>
+  </si>
+  <si>
+    <t>art activities</t>
+  </si>
+  <si>
+    <t>Bronzare organica</t>
+  </si>
+  <si>
+    <t>Chirurgie estetica</t>
+  </si>
+  <si>
+    <t>Coafor</t>
+  </si>
+  <si>
+    <t>Cosmetica</t>
+  </si>
+  <si>
+    <t>Epilare definitiva</t>
+  </si>
+  <si>
+    <t>Frizerie</t>
+  </si>
+  <si>
+    <t>Make-up</t>
+  </si>
+  <si>
+    <t>Manichiura</t>
+  </si>
+  <si>
+    <t>Masaj</t>
+  </si>
+  <si>
+    <t>Pedichiura</t>
+  </si>
+  <si>
+    <t>Remodelare corporala</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>Spa</t>
+  </si>
+  <si>
+    <t>Tatuaje&amp;piercing</t>
+  </si>
+  <si>
+    <t>Domeniul asociat</t>
+  </si>
+  <si>
+    <t>Serviciu</t>
+  </si>
+  <si>
+    <t>Durata serviciu</t>
+  </si>
+  <si>
+    <t>Pret serviciu</t>
+  </si>
+  <si>
+    <t>Persoane serviciu</t>
+  </si>
+  <si>
+    <t>teme acasa</t>
+  </si>
+  <si>
+    <t>darts</t>
+  </si>
+  <si>
+    <t>pictura</t>
+  </si>
+  <si>
+    <t>jocuri logica</t>
+  </si>
+  <si>
+    <t>100.66</t>
+  </si>
+  <si>
+    <t>Nume angajat</t>
+  </si>
+  <si>
+    <t>Email angajat</t>
+  </si>
+  <si>
+    <t>Telefon angajat</t>
+  </si>
+  <si>
+    <t>Serviciu asignat</t>
+  </si>
+  <si>
+    <t>Scolpol Maria</t>
+  </si>
+  <si>
+    <t>elenaz114a1@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0264555112</t>
+  </si>
+  <si>
+    <t>9:00-13:00</t>
+  </si>
+  <si>
+    <t>10:00-17:00</t>
+  </si>
+  <si>
+    <t>Mobutu seseku</t>
+  </si>
+  <si>
+    <t>komornicza11124@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0264111887</t>
+  </si>
+  <si>
+    <t>Moceal Rapil</t>
+  </si>
+  <si>
+    <t>ovidiusz11a34@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0265444112</t>
+  </si>
+  <si>
+    <t>Spiral Agar</t>
+  </si>
+  <si>
+    <t>sdrosea1sz4@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>10:00-21:00</t>
+  </si>
+  <si>
+    <t>9:00-18:30</t>
+  </si>
+  <si>
+    <t>Creare programari</t>
+  </si>
+  <si>
+    <t>Modificari programari in viitor</t>
+  </si>
+  <si>
+    <t>Modificari programari in trecut</t>
+  </si>
+  <si>
+    <t>Vizualizare calendar</t>
+  </si>
+  <si>
+    <t>Creare programari alti specialisti</t>
+  </si>
+  <si>
+    <t>Modificari programari in viitor alti specialisti</t>
+  </si>
+  <si>
+    <t>Modificari programari in trecut alti specialisti</t>
+  </si>
+  <si>
+    <t>Date de contact clienti</t>
+  </si>
+  <si>
+    <t>Vizualizare baza de date clienti</t>
+  </si>
+  <si>
+    <t>Editare informatii clienti</t>
+  </si>
+  <si>
+    <t>Setari orar</t>
+  </si>
+  <si>
+    <t>Setari exceptii</t>
   </si>
 </sst>
 </file>
@@ -835,7 +838,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
@@ -1034,7 +1037,6 @@
         <family val="2"/>
         <color rgb="FF000000"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -1125,11 +1127,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.35627530364373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1328,10 +1329,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.8097165991903"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.35627530364373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.3316326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1402,12 +1403,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.35627530364373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,9 +1587,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.35627530364373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1688,7 +1689,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.35627530364373"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,13 +1847,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.35627530364373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1977,14 +1976,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.6720647773279"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="0" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.35627530364373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2187,7 +2184,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
deleted staff email verification during business creation d
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cont adminstrator" sheetId="1" state="visible" r:id="rId2"/>
@@ -109,6 +109,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -197,6 +198,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -285,6 +287,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -311,7 +314,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Domeniu principal</t>
+          <t xml:space="preserve">Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -335,7 +338,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Domeniu principal</t>
+          <t xml:space="preserve">Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -349,7 +352,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Domeniu principal</t>
+          <t xml:space="preserve">Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -363,7 +366,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>*serviciile trebuie sa apartina neaparat de un domeniu</t>
+          <t xml:space="preserve">*serviciile trebuie sa apartina neaparat de un domeniu</t>
         </r>
       </text>
     </comment>
@@ -387,7 +390,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>* se pot adauga oricate conturi de angajati doriti</t>
+          <t xml:space="preserve">* se pot adauga oricate conturi de angajati doriti</t>
         </r>
       </text>
     </comment>
@@ -398,439 +401,439 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="145">
   <si>
-    <t>Categorie Afacere</t>
-  </si>
-  <si>
-    <t>Nume Afacere</t>
-  </si>
-  <si>
-    <t>Email Cont Administrator</t>
-  </si>
-  <si>
-    <t>Adresa afacere</t>
-  </si>
-  <si>
-    <t>Telefon afacere</t>
-  </si>
-  <si>
-    <t>Medicină dentară</t>
-  </si>
-  <si>
-    <t>Frumusețe</t>
-  </si>
-  <si>
-    <t>Larissa's style</t>
-  </si>
-  <si>
-    <t>larissa@yopmail.com</t>
-  </si>
-  <si>
-    <t>Calea Martirilor 127</t>
-  </si>
-  <si>
-    <t>0263221114</t>
-  </si>
-  <si>
-    <t>Medicină</t>
-  </si>
-  <si>
-    <t>Animale de companie</t>
-  </si>
-  <si>
-    <t>Sport și agrement</t>
-  </si>
-  <si>
-    <t>Terapii complementare</t>
-  </si>
-  <si>
-    <t>Auto</t>
-  </si>
-  <si>
-    <t>Instalații</t>
-  </si>
-  <si>
-    <t>Regomart</t>
-  </si>
-  <si>
-    <t>regomart@yopmail.com</t>
-  </si>
-  <si>
-    <t>Piata Mare 45</t>
-  </si>
-  <si>
-    <t>0264555113</t>
-  </si>
-  <si>
-    <t>Juridic</t>
-  </si>
-  <si>
-    <t>Resurse umane</t>
-  </si>
-  <si>
-    <t>Asigurări</t>
-  </si>
-  <si>
-    <t>Modă și îmbrăcăminte</t>
-  </si>
-  <si>
-    <t>Organizare evenimente</t>
-  </si>
-  <si>
-    <t>Educație</t>
-  </si>
-  <si>
-    <t>Scoala particulara Mario M</t>
-  </si>
-  <si>
-    <t>marioscaola1@automation.33mail.com</t>
-  </si>
-  <si>
-    <t>str Morariei nr 10</t>
-  </si>
-  <si>
-    <t>0264888641</t>
-  </si>
-  <si>
-    <t>Imobiliare</t>
-  </si>
-  <si>
-    <t>Bebeco Adeco</t>
-  </si>
-  <si>
-    <t>bebbeco@yopmail.com</t>
-  </si>
-  <si>
-    <t>Aleea Bucura 46</t>
-  </si>
-  <si>
-    <t>0254888777</t>
-  </si>
-  <si>
-    <t>Reparații</t>
-  </si>
-  <si>
-    <t>Psihologie</t>
-  </si>
-  <si>
-    <t>Altă categorie</t>
-  </si>
-  <si>
-    <t>Nume receptionist</t>
-  </si>
-  <si>
-    <t>Email receptionist</t>
-  </si>
-  <si>
-    <t>Telefon receptionist</t>
-  </si>
-  <si>
-    <t>Rubarba Mihaelaa</t>
-  </si>
-  <si>
-    <t>steluta2za1@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t>0264555887</t>
-  </si>
-  <si>
-    <t>Venula Mihaila</t>
-  </si>
-  <si>
-    <t>steluta3131zzdda@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t>0261111222</t>
-  </si>
-  <si>
-    <t>NilaStefania</t>
-  </si>
-  <si>
-    <t>steluta441za@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t>0268774112</t>
-  </si>
-  <si>
-    <t>Adresa locatie</t>
-  </si>
-  <si>
-    <t>Judet locatie</t>
-  </si>
-  <si>
-    <t>Localitate locatie</t>
-  </si>
-  <si>
-    <t>Telefon locatie</t>
-  </si>
-  <si>
-    <t>Nume locatie</t>
-  </si>
-  <si>
-    <t>Luni</t>
-  </si>
-  <si>
-    <t>Marti</t>
-  </si>
-  <si>
-    <t>Miercuri</t>
-  </si>
-  <si>
-    <t>Joi</t>
-  </si>
-  <si>
-    <t>Vineri</t>
-  </si>
-  <si>
-    <t>Sambata</t>
-  </si>
-  <si>
-    <t>Duminica</t>
-  </si>
-  <si>
-    <t>Str Fraternitatii nr 7</t>
-  </si>
-  <si>
-    <t>Cluj</t>
-  </si>
-  <si>
-    <t>Cluj-Napoca</t>
-  </si>
-  <si>
-    <t>0264555141</t>
-  </si>
-  <si>
-    <t>Sediu Flying</t>
-  </si>
-  <si>
-    <t>10:00-20:00</t>
-  </si>
-  <si>
-    <t>10:00-14:00</t>
-  </si>
-  <si>
-    <t>inchis</t>
-  </si>
-  <si>
-    <t>str Coloar 89</t>
-  </si>
-  <si>
-    <t>Alba</t>
-  </si>
-  <si>
-    <t>Alba Iulia</t>
-  </si>
-  <si>
-    <t>0263555441</t>
-  </si>
-  <si>
-    <t>Sediu Alba</t>
-  </si>
-  <si>
-    <t>9:00-17:00</t>
-  </si>
-  <si>
-    <t>9:00-21:00</t>
-  </si>
-  <si>
-    <t>9:00-15:00</t>
-  </si>
-  <si>
-    <t>str Alexadru Mircea nr 69</t>
-  </si>
-  <si>
-    <t>0254111222</t>
-  </si>
-  <si>
-    <t>Sediu Romulus</t>
-  </si>
-  <si>
-    <t>9:00-12:00</t>
-  </si>
-  <si>
-    <t>10:00-19:00</t>
-  </si>
-  <si>
-    <t>10:00-18:00</t>
-  </si>
-  <si>
-    <t>Nume domeniu</t>
-  </si>
-  <si>
-    <t>Locatia domeniului</t>
-  </si>
-  <si>
-    <t>scoala</t>
-  </si>
-  <si>
-    <t>playing</t>
-  </si>
-  <si>
-    <t>art activities</t>
-  </si>
-  <si>
-    <t>Bronzare organica</t>
-  </si>
-  <si>
-    <t>Chirurgie estetica</t>
-  </si>
-  <si>
-    <t>Coafor</t>
-  </si>
-  <si>
-    <t>Cosmetica</t>
-  </si>
-  <si>
-    <t>Epilare definitiva</t>
-  </si>
-  <si>
-    <t>Frizerie</t>
-  </si>
-  <si>
-    <t>Make-up</t>
-  </si>
-  <si>
-    <t>Manichiura</t>
-  </si>
-  <si>
-    <t>Masaj</t>
-  </si>
-  <si>
-    <t>Pedichiura</t>
-  </si>
-  <si>
-    <t>Remodelare corporala</t>
-  </si>
-  <si>
-    <t>Solar</t>
-  </si>
-  <si>
-    <t>Spa</t>
-  </si>
-  <si>
-    <t>Tatuaje&amp;piercing</t>
-  </si>
-  <si>
-    <t>Domeniul asociat</t>
-  </si>
-  <si>
-    <t>Serviciu</t>
-  </si>
-  <si>
-    <t>Durata serviciu</t>
-  </si>
-  <si>
-    <t>Pret serviciu</t>
-  </si>
-  <si>
-    <t>Persoane serviciu</t>
-  </si>
-  <si>
-    <t>teme acasa</t>
-  </si>
-  <si>
-    <t>darts</t>
-  </si>
-  <si>
-    <t>pictura</t>
-  </si>
-  <si>
-    <t>jocuri logica</t>
-  </si>
-  <si>
-    <t>100.66</t>
-  </si>
-  <si>
-    <t>Nume angajat</t>
-  </si>
-  <si>
-    <t>Email angajat</t>
-  </si>
-  <si>
-    <t>Telefon angajat</t>
-  </si>
-  <si>
-    <t>Serviciu asignat</t>
-  </si>
-  <si>
-    <t>Scolpol Maria</t>
-  </si>
-  <si>
-    <t>elenaz114a1@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t>0264555112</t>
-  </si>
-  <si>
-    <t>9:00-13:00</t>
-  </si>
-  <si>
-    <t>10:00-17:00</t>
-  </si>
-  <si>
-    <t>Mobutu seseku</t>
-  </si>
-  <si>
-    <t>komornicza11124@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t>0264111887</t>
-  </si>
-  <si>
-    <t>Moceal Rapil</t>
-  </si>
-  <si>
-    <t>ovidiusz11a34@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t>0265444112</t>
-  </si>
-  <si>
-    <t>Spiral Agar</t>
-  </si>
-  <si>
-    <t>sdrosea1sz4@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t>10:00-21:00</t>
-  </si>
-  <si>
-    <t>9:00-18:30</t>
-  </si>
-  <si>
-    <t>Creare programari</t>
-  </si>
-  <si>
-    <t>Modificari programari in viitor</t>
-  </si>
-  <si>
-    <t>Modificari programari in trecut</t>
-  </si>
-  <si>
-    <t>Vizualizare calendar</t>
-  </si>
-  <si>
-    <t>Creare programari alti specialisti</t>
-  </si>
-  <si>
-    <t>Modificari programari in viitor alti specialisti</t>
-  </si>
-  <si>
-    <t>Modificari programari in trecut alti specialisti</t>
-  </si>
-  <si>
-    <t>Date de contact clienti</t>
-  </si>
-  <si>
-    <t>Vizualizare baza de date clienti</t>
-  </si>
-  <si>
-    <t>Editare informatii clienti</t>
-  </si>
-  <si>
-    <t>Setari orar</t>
-  </si>
-  <si>
-    <t>Setari exceptii</t>
+    <t xml:space="preserve">Categorie Afacere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nume Afacere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email Cont Administrator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adresa afacere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telefon afacere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medicină dentară</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frumusețe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Larissa's style</t>
+  </si>
+  <si>
+    <t xml:space="preserve">larissa@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calea Martirilor 127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0263221114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medicină</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animale de companie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sport și agrement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terapii complementare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instalații</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regomart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regomart@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piata Mare 45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0264555113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juridic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resurse umane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asigurări</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modă și îmbrăcăminte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organizare evenimente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Educație</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scoala particulara SonyaM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sonyiacaola1@automation.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">str Morariei nr 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0264888641</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imobiliare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bebeco Adeco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bebbeco@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aleea Bucura 46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0254888777</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reparații</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Psihologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altă categorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nume receptionist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email receptionist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telefon receptionist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rubarba Mihaelaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">steluta2za1@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0264555887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venula Mihaila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">steluta3131zzdda@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0261111222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NilaStefania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">steluta441za@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0268774112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adresa locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Judet locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Localitate locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telefon locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nume locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miercuri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vineri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sambata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duminica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Str Fraternitatii nr 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluj-Napoca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0264555141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sediu Flying</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00-20:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00-14:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inchis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">str Coloar 89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alba Iulia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0263555441</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sediu Alba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-17:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-21:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-15:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">str Alexadru Mircea nr 69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0254111222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sediu Romulus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-12:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00-19:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00-18:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nume domeniu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locatia domeniului</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scoala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">playing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">art activities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bronzare organica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chirurgie estetica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coafor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cosmetica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epilare definitiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frizerie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manichiura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masaj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedichiura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remodelare corporala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tatuaje&amp;piercing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domeniul asociat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serviciu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Durata serviciu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pret serviciu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Persoane serviciu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teme acasa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">darts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pictura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jocuri logica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100.66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nume angajat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email angajat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telefon angajat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serviciu asignat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scolpol Maria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elenazzeta11@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0264555112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-13:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00-17:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobutu seseku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">komornicza11124@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0264111887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moceal Rapil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ovidiusz11a34@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0265444112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spiral Agar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdrosea1sz4@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00-21:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-18:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creare programari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modificari programari in viitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modificari programari in trecut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vizualizare calendar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creare programari alti specialisti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modificari programari in viitor alti specialisti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modificari programari in trecut alti specialisti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date de contact clienti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vizualizare baza de date clienti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editare informatii clienti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setari orar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setari exceptii</t>
   </si>
 </sst>
 </file>
@@ -838,7 +841,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
@@ -1037,6 +1040,7 @@
         <family val="2"/>
         <color rgb="FF000000"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -1127,10 +1131,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3562753036437"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.35627530364373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1323,16 +1327,16 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.3316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1403,12 +1407,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1587,9 +1591,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,7 +1693,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1847,11 +1851,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.10526315789474"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1970,18 +1976,18 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.35627530364373"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2184,7 +2190,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.35627530364373"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
new test data xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
@@ -110,6 +110,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -199,6 +200,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -288,6 +290,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -482,10 +485,10 @@
     <t xml:space="preserve">Educație</t>
   </si>
   <si>
-    <t xml:space="preserve">Scoala particulara SonyaM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sonyiacaola1@automation.33mail.com</t>
+    <t xml:space="preserve">Scoala particulara Miranda D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mirandascoalaa1@automation.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">str Morariei nr 10</t>
@@ -530,7 +533,7 @@
     <t xml:space="preserve">Rubarba Mihaelaa</t>
   </si>
   <si>
-    <t xml:space="preserve">steluta2za1@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">artoise23@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264555887</t>
@@ -539,7 +542,7 @@
     <t xml:space="preserve">Venula Mihaila</t>
   </si>
   <si>
-    <t xml:space="preserve">steluta3131zzdda@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">artemisa5@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0261111222</t>
@@ -548,7 +551,7 @@
     <t xml:space="preserve">NilaStefania</t>
   </si>
   <si>
-    <t xml:space="preserve">steluta441za@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">goblins1@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0268774112</t>
@@ -758,7 +761,7 @@
     <t xml:space="preserve">Scolpol Maria</t>
   </si>
   <si>
-    <t xml:space="preserve">elenazzeta11@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">fantastricarep@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264555112</t>
@@ -773,7 +776,7 @@
     <t xml:space="preserve">Mobutu seseku</t>
   </si>
   <si>
-    <t xml:space="preserve">komornicza11124@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">demokratiks4@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264111887</t>
@@ -782,7 +785,7 @@
     <t xml:space="preserve">Moceal Rapil</t>
   </si>
   <si>
-    <t xml:space="preserve">ovidiusz11a34@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">zanzibara@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0265444112</t>
@@ -791,7 +794,7 @@
     <t xml:space="preserve">Spiral Agar</t>
   </si>
   <si>
-    <t xml:space="preserve">sdrosea1sz4@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">zebralda@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">10:00-21:00</t>
@@ -1126,14 +1129,14 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -1328,14 +1331,14 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.7044534412956"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.0242914979757"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -1407,11 +1410,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.74898785425101"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -1591,8 +1594,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -1851,8 +1854,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.57085020242915"/>
@@ -1977,16 +1980,16 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
updated test data xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cont adminstrator" sheetId="1" state="visible" r:id="rId2"/>
@@ -115,6 +115,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -209,6 +210,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -303,6 +305,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -497,10 +500,10 @@
     <t xml:space="preserve">Educație</t>
   </si>
   <si>
-    <t xml:space="preserve">Scoala particulara Sbrownies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brownies@automation.33mail.com</t>
+    <t xml:space="preserve">Scoala particulara Little angels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">littleangel@automation.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">str Morariei nr 10</t>
@@ -545,7 +548,7 @@
     <t xml:space="preserve">Rubarba Mihaelaa</t>
   </si>
   <si>
-    <t xml:space="preserve">suzanna@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">suzanna1@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264555887</t>
@@ -554,7 +557,7 @@
     <t xml:space="preserve">Venula Mihaila</t>
   </si>
   <si>
-    <t xml:space="preserve">montana2@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">montana22@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0261111222</t>
@@ -563,7 +566,7 @@
     <t xml:space="preserve">NilaStefania</t>
   </si>
   <si>
-    <t xml:space="preserve">rimmelplus1@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">rimmelplus11@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0268774112</t>
@@ -773,7 +776,7 @@
     <t xml:space="preserve">Scolpol Maria</t>
   </si>
   <si>
-    <t xml:space="preserve">rasputind@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">rasputind2@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264555112</t>
@@ -788,7 +791,7 @@
     <t xml:space="preserve">Mobutu seseku</t>
   </si>
   <si>
-    <t xml:space="preserve">somailya@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">somailya2@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264111887</t>
@@ -797,7 +800,7 @@
     <t xml:space="preserve">Moceal Rapil</t>
   </si>
   <si>
-    <t xml:space="preserve">nigeria22@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">nigeria222@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0265444112</t>
@@ -806,7 +809,7 @@
     <t xml:space="preserve">Spiral Agar</t>
   </si>
   <si>
-    <t xml:space="preserve">otawau@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">otawau2@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">10:00-21:00</t>
@@ -1140,8 +1143,8 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1322,7 +1325,7 @@
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="larissa@yopmail.com"/>
     <hyperlink ref="C9" r:id="rId2" display="regomart@yopmail.com"/>
-    <hyperlink ref="C15" r:id="rId3" display="brownies@automation.33mail.com"/>
+    <hyperlink ref="C15" r:id="rId3" display="littleangel@automation.33mail.com"/>
     <hyperlink ref="C16" r:id="rId4" display="bebbeco@yopmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1349,9 +1352,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.8461538461538"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -1424,10 +1427,9 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -1608,7 +1610,7 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -1862,7 +1864,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1992,17 +1994,17 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8502024291498"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
updated test data xlsxc
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
@@ -117,6 +117,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -213,6 +215,8 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -309,6 +313,8 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -503,13 +509,13 @@
     <t xml:space="preserve">Educație</t>
   </si>
   <si>
-    <t xml:space="preserve">Scoala particulara Little sunshine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sunshine@automation.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">str Morariei nr 10</t>
+    <t xml:space="preserve">Scoala particulara Little sunshine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sunnyhill@automation33.mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">str Morariei nr 101</t>
   </si>
   <si>
     <t xml:space="preserve">0264888641</t>
@@ -1147,7 +1153,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1328,7 +1334,7 @@
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="larissa@yopmail.com"/>
     <hyperlink ref="C9" r:id="rId2" display="regomart@yopmail.com"/>
-    <hyperlink ref="C15" r:id="rId3" display="sunshine@automation.33mail.com"/>
+    <hyperlink ref="C15" r:id="rId3" display="sunnyhill@automation33.mail.com"/>
     <hyperlink ref="C16" r:id="rId4" display="bebbeco@yopmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1355,9 +1361,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.2753036437247"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -1431,8 +1437,8 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -1613,7 +1619,7 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -2003,11 +2009,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.7085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
api tests for register and data driven
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cont adminstrator" sheetId="1" state="visible" r:id="rId2"/>
@@ -123,6 +123,24 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -225,6 +243,24 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -327,6 +363,24 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -438,7 +492,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="146">
   <si>
     <t xml:space="preserve">Categorie Afacere</t>
   </si>
@@ -518,198 +572,201 @@
     <t xml:space="preserve">Organizare evenimente</t>
   </si>
   <si>
+    <t xml:space="preserve">Moda si imbracaminte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scoala particulara Little piggie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">littlepiggie15@automation.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">str Morariei nr 101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0264888641</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imobiliare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bebeco Adeco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bebbeco@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aleea Bucura 46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0254888777</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reparații</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Psihologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altă categorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nume receptionist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email receptionist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telefon receptionist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rubarba Mihaelaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lilanna1@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0264555887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venula Mihaila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moraritza22@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0261111222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NilaStefania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rimmelplus1@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0268774112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adresa locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Judet locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Localitate locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telefon locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nume locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miercuri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vineri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sambata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duminica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Str Fraternitatii nr 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluj-Napoca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0264555141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sediu Flying</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00-20:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00-14:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inchis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">str Coloar 89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alba Iulia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0263555441</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sediu Alba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-17:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-21:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-15:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">str Alexadru Mircea nr 69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0254111222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sediu Romulus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-12:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00-19:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00-18:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nume domeniu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locatia domeniului</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scoala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">playing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">art activities</t>
+  </si>
+  <si>
     <t xml:space="preserve">Educație</t>
   </si>
   <si>
-    <t xml:space="preserve">Scoala particulara Little pork</t>
-  </si>
-  <si>
-    <t xml:space="preserve">littlepoerk@automation.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">str Morariei nr 101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264888641</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imobiliare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bebeco Adeco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bebbeco@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aleea Bucura 46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0254888777</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reparații</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Psihologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Altă categorie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume receptionist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email receptionist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon receptionist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rubarba Mihaelaa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lilanna1@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555887</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venula Mihaila</t>
-  </si>
-  <si>
-    <t xml:space="preserve">moraritza22@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0261111222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NilaStefania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rimmelplus1@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0268774112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adresa locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Judet locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Localitate locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miercuri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vineri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sambata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duminica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Str Fraternitatii nr 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cluj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cluj-Napoca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555141</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediu Flying</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-20:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-14:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inchis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">str Coloar 89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alba Iulia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0263555441</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediu Alba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-17:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-21:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-15:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">str Alexadru Mircea nr 69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0254111222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediu Romulus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-12:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-19:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-18:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume domeniu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Locatia domeniului</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scoala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">playing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">art activities</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bronzare organica</t>
   </si>
   <si>
@@ -797,7 +854,7 @@
     <t xml:space="preserve">Scolpol Maria</t>
   </si>
   <si>
-    <t xml:space="preserve">raspbunty2@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">marilenaben6@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264555112</t>
@@ -812,7 +869,7 @@
     <t xml:space="preserve">Mobutu seseku</t>
   </si>
   <si>
-    <t xml:space="preserve">guineeas2@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">ideaforkih2@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264111887</t>
@@ -821,7 +878,7 @@
     <t xml:space="preserve">Moceal Rapil</t>
   </si>
   <si>
-    <t xml:space="preserve">nbegin4s2@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">boomsie4s2@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0265444112</t>
@@ -830,7 +887,7 @@
     <t xml:space="preserve">Spiral Agar</t>
   </si>
   <si>
-    <t xml:space="preserve">ocanrys2@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">ocarinass2@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">10:00-21:00</t>
@@ -1164,8 +1221,8 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1283,7 +1340,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1346,8 +1403,7 @@
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="larissa@yopmail.com"/>
     <hyperlink ref="C9" r:id="rId2" display="regomart@yopmail.com"/>
-    <hyperlink ref="C15" r:id="rId3" display="littlepoerk@automation.33mail.com"/>
-    <hyperlink ref="C16" r:id="rId4" display="bebbeco@yopmail.com"/>
+    <hyperlink ref="C16" r:id="rId3" display="bebbeco@yopmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1356,7 +1412,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1373,8 +1429,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.1295546558704"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.1417004048583"/>
   </cols>
@@ -1442,7 +1498,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+      <selection pane="topLeft" activeCell="M28" activeCellId="0" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1450,7 +1506,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -1631,7 +1687,7 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -1776,7 +1832,7 @@
         <v>25</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="O1" s="10" t="s">
         <v>31</v>
@@ -1790,72 +1846,72 @@
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1901,19 +1957,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1921,7 +1977,7 @@
         <v>87</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>30</v>
@@ -1938,7 +1994,7 @@
         <v>88</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>30</v>
@@ -1955,7 +2011,7 @@
         <v>89</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>20</v>
@@ -1972,13 +2028,13 @@
         <v>87</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>60</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E5" s="12" t="n">
         <v>1</v>
@@ -2015,14 +2071,14 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.4898785425101"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3886639676113"/>
@@ -2031,13 +2087,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>56</v>
@@ -2061,33 +2117,33 @@
         <v>62</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>76</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>76</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>76</v>
@@ -2096,18 +2152,18 @@
         <v>70</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>76</v>
@@ -2131,18 +2187,18 @@
         <v>70</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>76</v>
@@ -2166,42 +2222,42 @@
         <v>70</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J5" s="0" t="s">
         <v>70</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2234,192 +2290,192 @@
   <sheetData>
     <row r="1" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>